<commit_message>
add new updates do cpdb genes
</commit_message>
<xml_diff>
--- a/src/cellphonedb/summary/simple_significant_interactions_15_with_genes.xlsx
+++ b/src/cellphonedb/summary/simple_significant_interactions_15_with_genes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Imm.DAM.0" sheetId="1" state="visible" r:id="rId2"/>
@@ -884,7 +884,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
@@ -1170,7 +1170,7 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -1643,7 +1643,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -1890,7 +1890,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -2410,7 +2410,7 @@
       <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -2663,7 +2663,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -2859,11 +2859,18 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.09"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3201,16 +3208,16 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.5"/>
   </cols>
   <sheetData>

</xml_diff>